<commit_message>
Fatoração da classe GerarReembolsoFrame
</commit_message>
<xml_diff>
--- a/src/main/resources/com/meuprojeto/layout_preenchimento.xlsx
+++ b/src/main/resources/com/meuprojeto/layout_preenchimento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\ProjetosPessoais\automacao-reembolsos\src\main\resources\com\meuprojeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9260F70E-E282-4A80-AB5C-C6F5B770421B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC2BD5C-6079-40E5-A1F1-60BE62E63FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>RELATÓRIO DE DESPESAS</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">104 - CEF | Ag: 1525 | CC: 3225-7 </t>
+  </si>
+  <si>
+    <t>EXEMPLO</t>
   </si>
 </sst>
 </file>
@@ -432,9 +435,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,6 +500,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,10 +787,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,38 +806,38 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2"/>
@@ -854,11 +857,11 @@
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="25"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -872,110 +875,61 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="38">
+        <v>36526</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1000</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="12">
+        <f>SUM(C11:C11)</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="20">
+        <f ca="1">TODAY()</f>
+        <v>45794</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="21"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="13">
-        <f>SUM(C11:C22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="21">
-        <f ca="1">TODAY()</f>
-        <v>45793</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="22"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="23"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A25:B27"/>
-    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="A14:B16"/>
+    <mergeCell ref="C14:C16"/>
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" r:id="rId1"/>

</xml_diff>